<commit_message>
jira to ado script
</commit_message>
<xml_diff>
--- a/ado_project_details.xlsx
+++ b/ado_project_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
   <si>
     <t xml:space="preserve">Organization Name</t>
   </si>
@@ -44,9 +44,6 @@
   </si>
   <si>
     <t xml:space="preserve">demo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">koergsg5rol67lg7ulan63qxmu2fv3tz46fpqsme5cumqf2pkiha</t>
   </si>
   <si>
     <t xml:space="preserve">dhanushv@newtglobalcorp.com</t>
@@ -302,7 +299,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -329,7 +326,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -339,14 +336,12 @@
       <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="5"/>
+      <c r="E2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="3" customFormat="false" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -354,16 +349,14 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="4" customFormat="false" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -371,16 +364,14 @@
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="5" customFormat="false" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -388,13 +379,11 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="6" t="s">
         <v>8</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>